<commit_message>
Hoja con el promedio de credimiento
</commit_message>
<xml_diff>
--- a/05/AnalisisDatosI.xlsx
+++ b/05/AnalisisDatosI.xlsx
@@ -24,19 +24,32 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Año</t>
   </si>
   <si>
     <t>Población mundial</t>
   </si>
+  <si>
+    <t>% Crecimiento</t>
+  </si>
+  <si>
+    <t>Promedio últimos 30 años</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -73,29 +86,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -373,26 +391,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1000</v>
       </c>
@@ -400,156 +422,241 @@
         <v>410</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1650</v>
       </c>
       <c r="B3" s="2">
         <v>545</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" s="7">
+        <f>(B3/B2-1)/(A3-A2)</f>
+        <v>5.0656660412757985E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>1750</v>
       </c>
       <c r="B4" s="2">
         <v>791</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" s="7">
+        <f t="shared" ref="C4:C21" si="0">(B4/B3-1)/(A4-A3)</f>
+        <v>4.5137614678899072E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>1800</v>
       </c>
       <c r="B5" s="2">
         <v>981</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" s="7">
+        <f t="shared" si="0"/>
+        <v>4.8040455120101156E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>1850</v>
       </c>
       <c r="B6" s="3">
         <v>1262</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" s="7">
+        <f t="shared" si="0"/>
+        <v>5.7288481141692139E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>1900</v>
       </c>
       <c r="B7" s="3">
         <v>1650</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" s="7">
+        <f t="shared" si="0"/>
+        <v>6.1489698890649751E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>1950</v>
       </c>
       <c r="B8" s="3">
         <v>2516</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" s="7">
+        <f t="shared" si="0"/>
+        <v>1.0496969696969697E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>1955</v>
       </c>
       <c r="B9" s="3">
         <v>2751</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9" s="7">
+        <f t="shared" si="0"/>
+        <v>1.8680445151033398E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>1960</v>
       </c>
       <c r="B10" s="3">
         <v>3018</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10" s="7">
+        <f t="shared" si="0"/>
+        <v>1.9411123227917139E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>1965</v>
       </c>
       <c r="B11" s="3">
         <v>3335</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11" s="7">
+        <f t="shared" si="0"/>
+        <v>2.1007289595758795E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>1970</v>
       </c>
       <c r="B12" s="3">
         <v>3697</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12" s="7">
+        <f t="shared" si="0"/>
+        <v>2.1709145427286369E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>1975</v>
       </c>
       <c r="B13" s="3">
         <v>4077</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13" s="7">
+        <f t="shared" si="0"/>
+        <v>2.0557208547470916E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>1980</v>
       </c>
       <c r="B14" s="3">
         <v>4446</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14" s="7">
+        <f t="shared" si="0"/>
+        <v>1.8101545253863139E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>1985</v>
       </c>
       <c r="B15" s="3">
         <v>4854</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15" s="7">
+        <f t="shared" si="0"/>
+        <v>1.8353576248313085E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>1990</v>
       </c>
       <c r="B16" s="3">
         <v>5259</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" s="7">
+        <f t="shared" si="0"/>
+        <v>1.6687268232385664E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>1995</v>
       </c>
       <c r="B17" s="3">
         <v>5759</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" s="7">
+        <f t="shared" si="0"/>
+        <v>1.9015021867275151E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>2000</v>
       </c>
       <c r="B18" s="3">
         <v>6228</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18" s="7">
+        <f t="shared" si="0"/>
+        <v>1.6287549921861454E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>2005</v>
       </c>
       <c r="B19" s="3">
         <v>6574</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19" s="7">
+        <f t="shared" si="0"/>
+        <v>1.1111111111111117E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>2010</v>
       </c>
       <c r="B20" s="5">
         <v>6894</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20" s="7">
+        <f t="shared" si="0"/>
+        <v>9.7353209613629584E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>2015</v>
       </c>
       <c r="B21" s="5">
         <v>7349</v>
+      </c>
+      <c r="C21" s="7">
+        <f t="shared" si="0"/>
+        <v>1.3199883957064128E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" s="8">
+        <f>AVERAGE(C15:C21)</f>
+        <v>1.4912818899910505E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Añade el cálculo de población para 2015 con fórmula básica
</commit_message>
<xml_diff>
--- a/05/AnalisisDatosI.xlsx
+++ b/05/AnalisisDatosI.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Año</t>
   </si>
@@ -36,6 +36,9 @@
   </si>
   <si>
     <t>Promedio últimos 30 años</t>
+  </si>
+  <si>
+    <t>Previsión población 2016</t>
   </si>
 </sst>
 </file>
@@ -90,7 +93,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -107,9 +110,11 @@
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -391,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -410,7 +415,7 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
     </row>
@@ -429,7 +434,7 @@
       <c r="B3" s="2">
         <v>545</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="8">
         <f>(B3/B2-1)/(A3-A2)</f>
         <v>5.0656660412757985E-4</v>
       </c>
@@ -441,7 +446,7 @@
       <c r="B4" s="2">
         <v>791</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="8">
         <f t="shared" ref="C4:C21" si="0">(B4/B3-1)/(A4-A3)</f>
         <v>4.5137614678899072E-3</v>
       </c>
@@ -453,7 +458,7 @@
       <c r="B5" s="2">
         <v>981</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="8">
         <f t="shared" si="0"/>
         <v>4.8040455120101156E-3</v>
       </c>
@@ -465,7 +470,7 @@
       <c r="B6" s="3">
         <v>1262</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="8">
         <f t="shared" si="0"/>
         <v>5.7288481141692139E-3</v>
       </c>
@@ -477,7 +482,7 @@
       <c r="B7" s="3">
         <v>1650</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="8">
         <f t="shared" si="0"/>
         <v>6.1489698890649751E-3</v>
       </c>
@@ -489,7 +494,7 @@
       <c r="B8" s="3">
         <v>2516</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="8">
         <f t="shared" si="0"/>
         <v>1.0496969696969697E-2</v>
       </c>
@@ -501,7 +506,7 @@
       <c r="B9" s="3">
         <v>2751</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="8">
         <f t="shared" si="0"/>
         <v>1.8680445151033398E-2</v>
       </c>
@@ -513,7 +518,7 @@
       <c r="B10" s="3">
         <v>3018</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="8">
         <f t="shared" si="0"/>
         <v>1.9411123227917139E-2</v>
       </c>
@@ -525,7 +530,7 @@
       <c r="B11" s="3">
         <v>3335</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="8">
         <f t="shared" si="0"/>
         <v>2.1007289595758795E-2</v>
       </c>
@@ -537,7 +542,7 @@
       <c r="B12" s="3">
         <v>3697</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="8">
         <f t="shared" si="0"/>
         <v>2.1709145427286369E-2</v>
       </c>
@@ -549,7 +554,7 @@
       <c r="B13" s="3">
         <v>4077</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="8">
         <f t="shared" si="0"/>
         <v>2.0557208547470916E-2</v>
       </c>
@@ -561,7 +566,7 @@
       <c r="B14" s="3">
         <v>4446</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="8">
         <f t="shared" si="0"/>
         <v>1.8101545253863139E-2</v>
       </c>
@@ -573,7 +578,7 @@
       <c r="B15" s="3">
         <v>4854</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="8">
         <f t="shared" si="0"/>
         <v>1.8353576248313085E-2</v>
       </c>
@@ -585,7 +590,7 @@
       <c r="B16" s="3">
         <v>5259</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="8">
         <f t="shared" si="0"/>
         <v>1.6687268232385664E-2</v>
       </c>
@@ -597,7 +602,7 @@
       <c r="B17" s="3">
         <v>5759</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="8">
         <f t="shared" si="0"/>
         <v>1.9015021867275151E-2</v>
       </c>
@@ -609,7 +614,7 @@
       <c r="B18" s="3">
         <v>6228</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="8">
         <f t="shared" si="0"/>
         <v>1.6287549921861454E-2</v>
       </c>
@@ -621,7 +626,7 @@
       <c r="B19" s="3">
         <v>6574</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C19" s="8">
         <f t="shared" si="0"/>
         <v>1.1111111111111117E-2</v>
       </c>
@@ -633,7 +638,7 @@
       <c r="B20" s="5">
         <v>6894</v>
       </c>
-      <c r="C20" s="7">
+      <c r="C20" s="8">
         <f t="shared" si="0"/>
         <v>9.7353209613629584E-3</v>
       </c>
@@ -645,18 +650,30 @@
       <c r="B21" s="5">
         <v>7349</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C21" s="8">
         <f t="shared" si="0"/>
         <v>1.3199883957064128E-2</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C23" s="8">
+      <c r="C23" s="9">
         <f>AVERAGE(C15:C21)</f>
         <v>1.4912818899910505E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>2016</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="6">
+        <f>B21*C23+B21</f>
+        <v>7458.5943060954423</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tabla de población con una variable
</commit_message>
<xml_diff>
--- a/05/AnalisisDatosI.xlsx
+++ b/05/AnalisisDatosI.xlsx
@@ -396,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,7 +595,7 @@
         <v>1.6687268232385664E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>1995</v>
       </c>
@@ -607,7 +607,7 @@
         <v>1.9015021867275151E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>2000</v>
       </c>
@@ -619,7 +619,7 @@
         <v>1.6287549921861454E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>2005</v>
       </c>
@@ -631,7 +631,7 @@
         <v>1.1111111111111117E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>2010</v>
       </c>
@@ -643,7 +643,7 @@
         <v>9.7353209613629584E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>2015</v>
       </c>
@@ -655,7 +655,7 @@
         <v>1.3199883957064128E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B23" s="7" t="s">
         <v>3</v>
       </c>
@@ -664,16 +664,49 @@
         <v>1.4912818899910505E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2016</v>
       </c>
       <c r="B25" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C25" s="6">
+      <c r="D25" s="6">
         <f>B21*C23+B21</f>
         <v>7458.5943060954423</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C26" s="8">
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="D26" s="6">
+        <f t="dataTable" ref="D26:D29" dt2D="0" dtr="0" r1="C23"/>
+        <v>7440.8625000000002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C27" s="8">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D27" s="6">
+        <v>7459.2349999999997</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C28" s="8">
+        <v>1.7500000000000002E-2</v>
+      </c>
+      <c r="D28" s="6">
+        <v>7477.6075000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C29" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="D29" s="6">
+        <v>7495.98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tabla de población con dos variables
</commit_message>
<xml_diff>
--- a/05/AnalisisDatosI.xlsx
+++ b/05/AnalisisDatosI.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Año</t>
   </si>
@@ -39,6 +39,21 @@
   </si>
   <si>
     <t>Previsión población 2016</t>
+  </si>
+  <si>
+    <t>África</t>
+  </si>
+  <si>
+    <t>América</t>
+  </si>
+  <si>
+    <t>Asia</t>
+  </si>
+  <si>
+    <t>Europa</t>
+  </si>
+  <si>
+    <t>Oceanía</t>
   </si>
 </sst>
 </file>
@@ -93,7 +108,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -115,6 +130,9 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -396,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,7 +613,7 @@
         <v>1.6687268232385664E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>1995</v>
       </c>
@@ -607,7 +625,7 @@
         <v>1.9015021867275151E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>2000</v>
       </c>
@@ -619,7 +637,7 @@
         <v>1.6287549921861454E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>2005</v>
       </c>
@@ -631,7 +649,7 @@
         <v>1.1111111111111117E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>2010</v>
       </c>
@@ -643,7 +661,7 @@
         <v>9.7353209613629584E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>2015</v>
       </c>
@@ -655,7 +673,7 @@
         <v>1.3199883957064128E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B23" s="7" t="s">
         <v>3</v>
       </c>
@@ -664,49 +682,129 @@
         <v>1.4912818899910505E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D24" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H24" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2016</v>
       </c>
       <c r="B25" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D25" s="6">
+      <c r="C25" s="6">
         <f>B21*C23+B21</f>
         <v>7458.5943060954423</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D25" s="6">
+        <v>766621</v>
+      </c>
+      <c r="E25" s="6">
+        <v>818445</v>
+      </c>
+      <c r="F25" s="6">
+        <v>3634380</v>
+      </c>
+      <c r="G25" s="6">
+        <v>739508</v>
+      </c>
+      <c r="H25" s="6">
+        <v>30015</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C26" s="8">
         <v>1.2500000000000001E-2</v>
       </c>
       <c r="D26" s="6">
-        <f t="dataTable" ref="D26:D29" dt2D="0" dtr="0" r1="C23"/>
-        <v>7440.8625000000002</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="dataTable" ref="D26:H29" dt2D="1" dtr="1" r1="B21" r2="C23"/>
+        <v>776203.76249999995</v>
+      </c>
+      <c r="E26" s="6">
+        <v>828675.5625</v>
+      </c>
+      <c r="F26" s="6">
+        <v>3679809.75</v>
+      </c>
+      <c r="G26" s="6">
+        <v>748751.85</v>
+      </c>
+      <c r="H26" s="6">
+        <v>30390.1875</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C27" s="8">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="D27" s="6">
-        <v>7459.2349999999997</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+        <v>778120.31499999994</v>
+      </c>
+      <c r="E27" s="6">
+        <v>830721.67500000005</v>
+      </c>
+      <c r="F27" s="6">
+        <v>3688895.7</v>
+      </c>
+      <c r="G27" s="6">
+        <v>750600.62</v>
+      </c>
+      <c r="H27" s="6">
+        <v>30465.224999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C28" s="8">
         <v>1.7500000000000002E-2</v>
       </c>
       <c r="D28" s="6">
-        <v>7477.6075000000001</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+        <v>780036.86750000005</v>
+      </c>
+      <c r="E28" s="6">
+        <v>832767.78749999998</v>
+      </c>
+      <c r="F28" s="6">
+        <v>3697981.65</v>
+      </c>
+      <c r="G28" s="6">
+        <v>752449.39</v>
+      </c>
+      <c r="H28" s="6">
+        <v>30540.262500000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C29" s="8">
         <v>0.02</v>
       </c>
       <c r="D29" s="6">
-        <v>7495.98</v>
+        <v>781953.42</v>
+      </c>
+      <c r="E29" s="6">
+        <v>834813.9</v>
+      </c>
+      <c r="F29" s="6">
+        <v>3707067.6</v>
+      </c>
+      <c r="G29" s="6">
+        <v>754298.16</v>
+      </c>
+      <c r="H29" s="6">
+        <v>30615.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Hoja con datos con estacionalidad para previsiones
</commit_message>
<xml_diff>
--- a/05/AnalisisDatosI.xlsx
+++ b/05/AnalisisDatosI.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18105" windowHeight="10245"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18105" windowHeight="10245" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Historico población" sheetId="1" r:id="rId1"/>
+    <sheet name="Estacionalidad" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Año</t>
   </si>
@@ -54,6 +55,33 @@
   </si>
   <si>
     <t>Oceanía</t>
+  </si>
+  <si>
+    <t>Crecimiento</t>
+  </si>
+  <si>
+    <t>Pronóstico con suavizado</t>
+  </si>
+  <si>
+    <t>Pronóstico lineal</t>
+  </si>
+  <si>
+    <t>Intervalo de confianza</t>
+  </si>
+  <si>
+    <t>-Intervalo</t>
+  </si>
+  <si>
+    <t>+Intervalo</t>
+  </si>
+  <si>
+    <t>Temporalidad</t>
+  </si>
+  <si>
+    <t>Fechas</t>
+  </si>
+  <si>
+    <t>Valores</t>
   </si>
 </sst>
 </file>
@@ -108,7 +136,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -133,6 +161,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -414,16 +445,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -807,6 +840,281 @@
         <v>30615.3</v>
       </c>
     </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>2020</v>
+      </c>
+      <c r="B31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" s="6">
+        <f>FORECAST(A31,B8:B21,A8:A21)</f>
+        <v>7651.6703296703054</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32" s="6">
+        <f>GROWTH(B8:B21,A8:A21,A31)</f>
+        <v>8498.253995232275</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" s="6">
+        <f>_xlfn.FORECAST.ETS(A31,B8:B21,A8:A21)</f>
+        <v>7771.0663097859751</v>
+      </c>
+      <c r="D33" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E33" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="I33" s="13"/>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" s="6">
+        <f>_xlfn.FORECAST.ETS.CONFINT(A31,B8:B21,A8:A21,0.9)</f>
+        <v>124.7408412434021</v>
+      </c>
+      <c r="D34" s="6">
+        <f>C33-C34</f>
+        <v>7646.3254685425727</v>
+      </c>
+      <c r="E34" s="6">
+        <f>C33+C34</f>
+        <v>7895.8071510293776</v>
+      </c>
+      <c r="I34" s="13"/>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I35" s="13"/>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I36" s="13"/>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I37" s="13"/>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I38" s="13"/>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I39" s="13"/>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I40" s="13"/>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I41" s="13"/>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I42" s="13"/>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I43" s="13"/>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I44" s="13"/>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I45" s="13"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="C31:C34" formulaRange="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="13">
+        <v>42370</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="13">
+        <v>42371</v>
+      </c>
+      <c r="B3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="13">
+        <v>42372</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="13">
+        <v>42373</v>
+      </c>
+      <c r="B5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="13">
+        <v>42374</v>
+      </c>
+      <c r="B6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="13">
+        <v>42375</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="13">
+        <v>42376</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="13">
+        <v>42377</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="13">
+        <v>42378</v>
+      </c>
+      <c r="B10">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="13">
+        <v>42379</v>
+      </c>
+      <c r="B11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="13">
+        <v>42380</v>
+      </c>
+      <c r="B12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="13">
+        <v>42381</v>
+      </c>
+      <c r="B13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="13">
+        <v>42382</v>
+      </c>
+      <c r="B14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="13">
+        <v>42383</v>
+      </c>
+      <c r="B15" s="14">
+        <f>_xlfn.FORECAST.ETS(A15,B2:B14,A2:A14)</f>
+        <v>11.432426764461479</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="13">
+        <v>42384</v>
+      </c>
+      <c r="B16" s="14">
+        <f>_xlfn.FORECAST.ETS(A16,B$2:B$14,A$2:A$14)</f>
+        <v>12.869786853797208</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="13">
+        <v>42385</v>
+      </c>
+      <c r="B17" s="14">
+        <f>_xlfn.FORECAST.ETS(A17,B$2:B$14,A$2:A$14)</f>
+        <v>5.8770212261694663</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="13">
+        <v>42386</v>
+      </c>
+      <c r="B18" s="14">
+        <f>_xlfn.FORECAST.ETS(A18,B$2:B$14,A$2:A$14)</f>
+        <v>5.4147057006752171</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="13">
+        <v>42387</v>
+      </c>
+      <c r="B19" s="14">
+        <f>_xlfn.FORECAST.ETS(A19,B$2:B$14,A$2:A$14)</f>
+        <v>6.4179358004613523</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21">
+        <f>_xlfn.FORECAST.ETS.SEASONALITY(B2:B14,A2:A14)</f>
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Hoja con parámetros estadísticos del pronóstico
</commit_message>
<xml_diff>
--- a/05/AnalisisDatosI.xlsx
+++ b/05/AnalisisDatosI.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18105" windowHeight="10245" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18105" windowHeight="10245"/>
   </bookViews>
   <sheets>
     <sheet name="Historico población" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Año</t>
   </si>
@@ -82,13 +82,44 @@
   </si>
   <si>
     <t>Valores</t>
+  </si>
+  <si>
+    <t>ETS.STAT</t>
+  </si>
+  <si>
+    <t>Alfa</t>
+  </si>
+  <si>
+    <t>Beta</t>
+  </si>
+  <si>
+    <t>Gamma</t>
+  </si>
+  <si>
+    <t>MASE</t>
+  </si>
+  <si>
+    <t>SMAPE</t>
+  </si>
+  <si>
+    <t>MAE</t>
+  </si>
+  <si>
+    <t>ECM</t>
+  </si>
+  <si>
+    <t>Tamaño de paso</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="169" formatCode="0.000"/>
+    <numFmt numFmtId="173" formatCode="0.000E+00"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -97,6 +128,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -136,34 +175,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -447,8 +489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -861,7 +903,7 @@
         <v>8498.253995232275</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>11</v>
       </c>
@@ -877,7 +919,7 @@
       </c>
       <c r="I33" s="13"/>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>13</v>
       </c>
@@ -895,41 +937,101 @@
       </c>
       <c r="I34" s="13"/>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B35" t="s">
+        <v>20</v>
+      </c>
+      <c r="C35" s="14">
+        <f>_xlfn.FORECAST.ETS.STAT(B8:B21,A8:A21,1)</f>
+        <v>0.9</v>
+      </c>
       <c r="I35" s="13"/>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>21</v>
+      </c>
+      <c r="C36" s="14">
+        <f>_xlfn.FORECAST.ETS.STAT(B8:B21,A8:A21,2)</f>
+        <v>0.89900000000000002</v>
+      </c>
       <c r="I36" s="13"/>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>22</v>
+      </c>
+      <c r="C37" s="17">
+        <f>_xlfn.FORECAST.ETS.STAT(B8:B21,A8:A21,3)</f>
+        <v>2.2204460492503131E-16</v>
+      </c>
       <c r="I37" s="13"/>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>23</v>
+      </c>
+      <c r="C38" s="14">
+        <f>_xlfn.FORECAST.ETS.STAT(B8:B21,A8:A21,4)</f>
+        <v>0.25095768002045332</v>
+      </c>
       <c r="I38" s="13"/>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>24</v>
+      </c>
+      <c r="C39" s="14">
+        <f>_xlfn.FORECAST.ETS.STAT(B8:B21,A8:A21,5)</f>
+        <v>1.3007328337635182E-2</v>
+      </c>
       <c r="I39" s="13"/>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>25</v>
+      </c>
+      <c r="C40" s="14">
+        <f>_xlfn.FORECAST.ETS.STAT(B8:B21,A8:A21,6)</f>
+        <v>86.047114537012931</v>
+      </c>
       <c r="I40" s="13"/>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>26</v>
+      </c>
+      <c r="C41" s="14">
+        <f>_xlfn.FORECAST.ETS.STAT(B8:B21,A8:A21,7)</f>
+        <v>98.665633615509094</v>
+      </c>
       <c r="I41" s="13"/>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>27</v>
+      </c>
+      <c r="C42" s="14">
+        <f>_xlfn.FORECAST.ETS.STAT(B8:B21,A8:A21,8)</f>
+        <v>5</v>
+      </c>
       <c r="I42" s="13"/>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I43" s="13"/>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I44" s="13"/>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I45" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError sqref="C31:C34" formulaRange="1"/>
   </ignoredErrors>
@@ -940,7 +1042,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
@@ -1065,7 +1167,7 @@
       <c r="A15" s="13">
         <v>42383</v>
       </c>
-      <c r="B15" s="14">
+      <c r="B15" s="15">
         <f>_xlfn.FORECAST.ETS(A15,B2:B14,A2:A14)</f>
         <v>11.432426764461479</v>
       </c>
@@ -1074,7 +1176,7 @@
       <c r="A16" s="13">
         <v>42384</v>
       </c>
-      <c r="B16" s="14">
+      <c r="B16" s="15">
         <f>_xlfn.FORECAST.ETS(A16,B$2:B$14,A$2:A$14)</f>
         <v>12.869786853797208</v>
       </c>
@@ -1083,7 +1185,7 @@
       <c r="A17" s="13">
         <v>42385</v>
       </c>
-      <c r="B17" s="14">
+      <c r="B17" s="15">
         <f>_xlfn.FORECAST.ETS(A17,B$2:B$14,A$2:A$14)</f>
         <v>5.8770212261694663</v>
       </c>
@@ -1092,7 +1194,7 @@
       <c r="A18" s="13">
         <v>42386</v>
       </c>
-      <c r="B18" s="14">
+      <c r="B18" s="15">
         <f>_xlfn.FORECAST.ETS(A18,B$2:B$14,A$2:A$14)</f>
         <v>5.4147057006752171</v>
       </c>
@@ -1101,7 +1203,7 @@
       <c r="A19" s="13">
         <v>42387</v>
       </c>
-      <c r="B19" s="14">
+      <c r="B19" s="15">
         <f>_xlfn.FORECAST.ETS(A19,B$2:B$14,A$2:A$14)</f>
         <v>6.4179358004613523</v>
       </c>

</xml_diff>

<commit_message>
Hoja con resultados de previsión incluyendo gráfica
</commit_message>
<xml_diff>
--- a/05/AnalisisDatosI.xlsx
+++ b/05/AnalisisDatosI.xlsx
@@ -9,11 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18105" windowHeight="10245"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18105" windowHeight="10245" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Historico población" sheetId="1" r:id="rId1"/>
-    <sheet name="Estacionalidad" sheetId="2" r:id="rId2"/>
+    <sheet name="ResultadoPrevision" sheetId="4" r:id="rId2"/>
+    <sheet name="Prevision" sheetId="3" r:id="rId3"/>
+    <sheet name="Estacionalidad" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
   <si>
     <t>Año</t>
   </si>
@@ -109,6 +111,24 @@
   </si>
   <si>
     <t>Tamaño de paso</t>
+  </si>
+  <si>
+    <t>Previsión(Población mundial)</t>
+  </si>
+  <si>
+    <t>Intervalo de confianza(Población mundial)</t>
+  </si>
+  <si>
+    <t>Estadística</t>
+  </si>
+  <si>
+    <t>Valor</t>
+  </si>
+  <si>
+    <t>Alpha</t>
+  </si>
+  <si>
+    <t>RMSE</t>
   </si>
 </sst>
 </file>
@@ -175,7 +195,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -206,12 +226,28 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -222,6 +258,1089 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ResultadoPrevision!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Población mundial</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>ResultadoPrevision!$B$2:$B$19</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>2516</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2751</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3018</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3335</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3697</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4077</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4446</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4854</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5259</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5759</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6228</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6574</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6894</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7349</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8913-46C8-A4EF-C98FA748EC28}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ResultadoPrevision!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Previsión(Población mundial)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>ResultadoPrevision!$D$2:$D$19</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="18"/>
+                  <c:pt idx="14">
+                    <c:v>148.63788013248538</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>305.93420338845044</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>504.39745033763495</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>735.02918089286527</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>ResultadoPrevision!$D$2:$D$19</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="18"/>
+                  <c:pt idx="14">
+                    <c:v>148.63788013248538</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>305.93420338845044</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>504.39745033763495</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>735.02918089286527</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:srgbClr val="595959">
+                    <a:alpha val="40392"/>
+                  </a:srgbClr>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:numRef>
+              <c:f>ResultadoPrevision!$A$2:$A$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>1950</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1955</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1960</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1965</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1970</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1975</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1980</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1985</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1990</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1995</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2030</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2035</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ResultadoPrevision!$C$2:$C$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="14" formatCode="#,##0">
+                  <c:v>7771.0663097859751</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="#,##0">
+                  <c:v>8206.9396495397395</c:v>
+                </c:pt>
+                <c:pt idx="16" formatCode="#,##0">
+                  <c:v>8642.8129892935049</c:v>
+                </c:pt>
+                <c:pt idx="17" formatCode="#,##0">
+                  <c:v>9078.6863290472684</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8913-46C8-A4EF-C98FA748EC28}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="0"/>
+        <c:overlap val="100"/>
+        <c:axId val="464765088"/>
+        <c:axId val="464762136"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="464765088"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="464762136"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="464762136"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="464765088"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1681162</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>280987</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:D19" totalsRowShown="0">
+  <autoFilter ref="A1:D19"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Año" dataDxfId="3"/>
+    <tableColumn id="2" name="Población mundial"/>
+    <tableColumn id="3" name="Previsión(Población mundial)" dataDxfId="2">
+      <calculatedColumnFormula>_xlfn.FORECAST.ETS(A2,$B$2:$B$15,$A$2:$A$15,1,1)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" name="Intervalo de confianza(Población mundial)" dataDxfId="1">
+      <calculatedColumnFormula>_xlfn.FORECAST.ETS.CONFINT(A2,$B$2:$B$15,$A$2:$A$15,0.95,1,1)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="G1:H8" totalsRowShown="0">
+  <autoFilter ref="G1:H8"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Estadística"/>
+    <tableColumn id="2" name="Valor" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -489,8 +1608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1033,12 +2152,410 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="C31:C34" formulaRange="1"/>
+    <ignoredError sqref="C31:C42" formulaRange="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="19.5703125" customWidth="1"/>
+    <col min="3" max="3" width="29.28515625" customWidth="1"/>
+    <col min="4" max="4" width="40.5703125" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" customWidth="1"/>
+    <col min="8" max="8" width="7.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="18">
+        <v>1950</v>
+      </c>
+      <c r="B2" s="19">
+        <v>2516</v>
+      </c>
+      <c r="G2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" s="20">
+        <f>_xlfn.FORECAST.ETS.STAT($B$2:$B$15,$A$2:$A$15,1,1,1)</f>
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="18">
+        <v>1955</v>
+      </c>
+      <c r="B3" s="19">
+        <v>2751</v>
+      </c>
+      <c r="G3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="20">
+        <f>_xlfn.FORECAST.ETS.STAT($B$2:$B$15,$A$2:$A$15,2,1,1)</f>
+        <v>0.89900000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="18">
+        <v>1960</v>
+      </c>
+      <c r="B4" s="19">
+        <v>3018</v>
+      </c>
+      <c r="G4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="20">
+        <f>_xlfn.FORECAST.ETS.STAT($B$2:$B$15,$A$2:$A$15,3,1,1)</f>
+        <v>2.2204460492503131E-16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="18">
+        <v>1965</v>
+      </c>
+      <c r="B5" s="19">
+        <v>3335</v>
+      </c>
+      <c r="G5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="20">
+        <f>_xlfn.FORECAST.ETS.STAT($B$2:$B$15,$A$2:$A$15,4,1,1)</f>
+        <v>0.25095768002045332</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="18">
+        <v>1970</v>
+      </c>
+      <c r="B6" s="19">
+        <v>3697</v>
+      </c>
+      <c r="G6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" s="20">
+        <f>_xlfn.FORECAST.ETS.STAT($B$2:$B$15,$A$2:$A$15,5,1,1)</f>
+        <v>1.3007328337635182E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="18">
+        <v>1975</v>
+      </c>
+      <c r="B7" s="19">
+        <v>4077</v>
+      </c>
+      <c r="G7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="20">
+        <f>_xlfn.FORECAST.ETS.STAT($B$2:$B$15,$A$2:$A$15,6,1,1)</f>
+        <v>86.047114537012931</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="18">
+        <v>1980</v>
+      </c>
+      <c r="B8" s="19">
+        <v>4446</v>
+      </c>
+      <c r="G8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" s="20">
+        <f>_xlfn.FORECAST.ETS.STAT($B$2:$B$15,$A$2:$A$15,7,1,1)</f>
+        <v>98.665633615509094</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="18">
+        <v>1985</v>
+      </c>
+      <c r="B9" s="19">
+        <v>4854</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="18">
+        <v>1990</v>
+      </c>
+      <c r="B10" s="19">
+        <v>5259</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="18">
+        <v>1995</v>
+      </c>
+      <c r="B11" s="19">
+        <v>5759</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="18">
+        <v>2000</v>
+      </c>
+      <c r="B12" s="19">
+        <v>6228</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="18">
+        <v>2005</v>
+      </c>
+      <c r="B13" s="19">
+        <v>6574</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="18">
+        <v>2010</v>
+      </c>
+      <c r="B14" s="19">
+        <v>6894</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="18">
+        <v>2015</v>
+      </c>
+      <c r="B15" s="19">
+        <v>7349</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="18">
+        <v>2020</v>
+      </c>
+      <c r="C16" s="19">
+        <f>_xlfn.FORECAST.ETS(A16,$B$2:$B$15,$A$2:$A$15,1,1)</f>
+        <v>7771.0663097859751</v>
+      </c>
+      <c r="D16" s="19">
+        <f>_xlfn.FORECAST.ETS.CONFINT(A16,$B$2:$B$15,$A$2:$A$15,0.95,1,1)</f>
+        <v>148.63788013248538</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="18">
+        <v>2025</v>
+      </c>
+      <c r="C17" s="19">
+        <f>_xlfn.FORECAST.ETS(A17,$B$2:$B$15,$A$2:$A$15,1,1)</f>
+        <v>8206.9396495397395</v>
+      </c>
+      <c r="D17" s="19">
+        <f>_xlfn.FORECAST.ETS.CONFINT(A17,$B$2:$B$15,$A$2:$A$15,0.95,1,1)</f>
+        <v>305.93420338845044</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="18">
+        <v>2030</v>
+      </c>
+      <c r="C18" s="19">
+        <f>_xlfn.FORECAST.ETS(A18,$B$2:$B$15,$A$2:$A$15,1,1)</f>
+        <v>8642.8129892935049</v>
+      </c>
+      <c r="D18" s="19">
+        <f>_xlfn.FORECAST.ETS.CONFINT(A18,$B$2:$B$15,$A$2:$A$15,0.95,1,1)</f>
+        <v>504.39745033763495</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="18">
+        <v>2035</v>
+      </c>
+      <c r="C19" s="19">
+        <f>_xlfn.FORECAST.ETS(A19,$B$2:$B$15,$A$2:$A$15,1,1)</f>
+        <v>9078.6863290472684</v>
+      </c>
+      <c r="D19" s="19">
+        <f>_xlfn.FORECAST.ETS.CONFINT(A19,$B$2:$B$15,$A$2:$A$15,0.95,1,1)</f>
+        <v>735.02918089286527</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="2">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1950</v>
+      </c>
+      <c r="B2" s="3">
+        <v>2516</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>1955</v>
+      </c>
+      <c r="B3" s="3">
+        <v>2751</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>1960</v>
+      </c>
+      <c r="B4" s="3">
+        <v>3018</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>1965</v>
+      </c>
+      <c r="B5" s="3">
+        <v>3335</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>1970</v>
+      </c>
+      <c r="B6" s="3">
+        <v>3697</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>1975</v>
+      </c>
+      <c r="B7" s="3">
+        <v>4077</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>1980</v>
+      </c>
+      <c r="B8" s="3">
+        <v>4446</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>1985</v>
+      </c>
+      <c r="B9" s="3">
+        <v>4854</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>1990</v>
+      </c>
+      <c r="B10" s="3">
+        <v>5259</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>1995</v>
+      </c>
+      <c r="B11" s="3">
+        <v>5759</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>2000</v>
+      </c>
+      <c r="B12" s="3">
+        <v>6228</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>2005</v>
+      </c>
+      <c r="B13" s="3">
+        <v>6574</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>2010</v>
+      </c>
+      <c r="B14" s="5">
+        <v>6894</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>2015</v>
+      </c>
+      <c r="B15" s="5">
+        <v>7349</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B21"/>
   <sheetViews>

</xml_diff>

<commit_message>
Hoja con datos base para los esnarios
</commit_message>
<xml_diff>
--- a/05/AnalisisDatosI.xlsx
+++ b/05/AnalisisDatosI.xlsx
@@ -9,14 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18105" windowHeight="10245" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18105" windowHeight="10245" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Historico población" sheetId="1" r:id="rId1"/>
     <sheet name="ResultadoPrevision" sheetId="4" r:id="rId2"/>
     <sheet name="Prevision" sheetId="3" r:id="rId3"/>
     <sheet name="Estacionalidad" sheetId="2" r:id="rId4"/>
+    <sheet name="Escenarios" sheetId="5" r:id="rId5"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId6"/>
+  </externalReferences>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -27,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="34">
   <si>
     <t>Año</t>
   </si>
@@ -135,9 +139,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="169" formatCode="0.000"/>
     <numFmt numFmtId="173" formatCode="0.000E+00"/>
+    <numFmt numFmtId="174" formatCode="#,##0.00\ &quot;pta&quot;;[Red]\-#,##0.00\ &quot;pta&quot;"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -195,7 +200,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -229,6 +234,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="174" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1313,6 +1321,77 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Tablas de datos"/>
+      <sheetName val="Informe de respuestas"/>
+      <sheetName val="Informe de confidencialidad"/>
+      <sheetName val="Informe de límites"/>
+      <sheetName val="Escenarios"/>
+      <sheetName val="Estadística descriptiva"/>
+      <sheetName val="Histograma"/>
+      <sheetName val="Global"/>
+      <sheetName val="Tabla dinámica del escenario"/>
+      <sheetName val="Resumen de escenario"/>
+      <sheetName val="África"/>
+      <sheetName val="América"/>
+      <sheetName val="Asia"/>
+      <sheetName val="Europa"/>
+      <sheetName val="Oceanía"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1">
+        <row r="58">
+          <cell r="F58">
+            <v>766621</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="11" refreshError="1">
+        <row r="52">
+          <cell r="F52">
+            <v>818445</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="12" refreshError="1">
+        <row r="51">
+          <cell r="F51">
+            <v>3634280</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="13" refreshError="1">
+        <row r="47">
+          <cell r="F47">
+            <v>739508</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="14" refreshError="1">
+        <row r="25">
+          <cell r="F25">
+            <v>30015</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2161,7 +2240,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -2737,4 +2816,69 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:F5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="6">
+        <f>[1]África!F58</f>
+        <v>766621</v>
+      </c>
+      <c r="C4" s="6">
+        <f>[1]América!F52</f>
+        <v>818445</v>
+      </c>
+      <c r="D4" s="6">
+        <f>[1]Asia!F51</f>
+        <v>3634280</v>
+      </c>
+      <c r="E4" s="6">
+        <f>[1]Europa!F47</f>
+        <v>739508</v>
+      </c>
+      <c r="F4" s="6">
+        <f>[1]Oceanía!F25</f>
+        <v>30015</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
+        <v>1.52E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fórmulas y nombres de los datos base para los escenarios
</commit_message>
<xml_diff>
--- a/05/AnalisisDatosI.xlsx
+++ b/05/AnalisisDatosI.xlsx
@@ -21,6 +21,14 @@
   <externalReferences>
     <externalReference r:id="rId6"/>
   </externalReferences>
+  <definedNames>
+    <definedName name="Crecimiento">Escenarios!$A$5</definedName>
+    <definedName name="PoblacionAfrica">Escenarios!$B$5</definedName>
+    <definedName name="PoblacionAmerica">Escenarios!$C$5</definedName>
+    <definedName name="PoblacionAsia">Escenarios!$D$5</definedName>
+    <definedName name="PoblacionEuropa">Escenarios!$E$5</definedName>
+    <definedName name="PoblacionOceania">Escenarios!$F$5</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -2823,7 +2831,7 @@
   <dimension ref="A3:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2877,6 +2885,26 @@
       <c r="A5" s="8">
         <v>1.52E-2</v>
       </c>
+      <c r="B5" s="6">
+        <f>B4*Crecimiento+B4</f>
+        <v>778273.63919999998</v>
+      </c>
+      <c r="C5" s="6">
+        <f>C4*Crecimiento+C4</f>
+        <v>830885.36399999994</v>
+      </c>
+      <c r="D5" s="6">
+        <f>D4*Crecimiento+D4</f>
+        <v>3689521.0559999999</v>
+      </c>
+      <c r="E5" s="6">
+        <f>E4*Crecimiento+E4</f>
+        <v>750748.52159999998</v>
+      </c>
+      <c r="F5" s="6">
+        <f>F4*Crecimiento+F4</f>
+        <v>30471.227999999999</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Hoja con los tres escenarios de crecimiento definidos
</commit_message>
<xml_diff>
--- a/05/AnalisisDatosI.xlsx
+++ b/05/AnalisisDatosI.xlsx
@@ -2831,7 +2831,7 @@
   <dimension ref="A3:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2883,30 +2883,41 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
-        <v>1.52E-2</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="B5" s="6">
         <f>B4*Crecimiento+B4</f>
-        <v>778273.63919999998</v>
+        <v>770454.10499999998</v>
       </c>
       <c r="C5" s="6">
         <f>C4*Crecimiento+C4</f>
-        <v>830885.36399999994</v>
+        <v>822537.22499999998</v>
       </c>
       <c r="D5" s="6">
         <f>D4*Crecimiento+D4</f>
-        <v>3689521.0559999999</v>
+        <v>3652451.4</v>
       </c>
       <c r="E5" s="6">
         <f>E4*Crecimiento+E4</f>
-        <v>750748.52159999998</v>
+        <v>743205.54</v>
       </c>
       <c r="F5" s="6">
         <f>F4*Crecimiento+F4</f>
-        <v>30471.227999999999</v>
+        <v>30165.075000000001</v>
       </c>
     </row>
   </sheetData>
+  <scenarios current="0" show="2">
+    <scenario name="Crecimiento superior" locked="1" count="1" user="Francisco Charte Ojeda" comment="Creado por Francisco Charte Ojeda el 10/02/2016">
+      <inputCells r="A5" val="0,025" numFmtId="10"/>
+    </scenario>
+    <scenario name="Crecimiento promedio" locked="1" count="1" user="Francisco Charte Ojeda" comment="Creado por Francisco Charte Ojeda el 10/02/2016">
+      <inputCells r="A5" val="0,015" numFmtId="10"/>
+    </scenario>
+    <scenario name="Crecimiento inferior" locked="1" count="1" user="Francisco Charte Ojeda" comment="Creado por Francisco Charte Ojeda el 10/02/2016">
+      <inputCells r="A5" val="0,005" numFmtId="10"/>
+    </scenario>
+  </scenarios>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Hoja con resumen de los objetivos definidos
</commit_message>
<xml_diff>
--- a/05/AnalisisDatosI.xlsx
+++ b/05/AnalisisDatosI.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18105" windowHeight="10245" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18105" windowHeight="10245" firstSheet="4" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Historico población" sheetId="1" r:id="rId1"/>
@@ -17,9 +17,11 @@
     <sheet name="Prevision" sheetId="3" r:id="rId3"/>
     <sheet name="Estacionalidad" sheetId="2" r:id="rId4"/>
     <sheet name="Escenarios" sheetId="5" r:id="rId5"/>
+    <sheet name="Tabla dinámica del escenario" sheetId="6" r:id="rId6"/>
+    <sheet name="Resumen del escenario" sheetId="8" r:id="rId7"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId6"/>
+    <externalReference r:id="rId8"/>
   </externalReferences>
   <definedNames>
     <definedName name="Crecimiento">Escenarios!$A$5</definedName>
@@ -30,6 +32,9 @@
     <definedName name="PoblacionOceania">Escenarios!$F$5</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
+  <pivotCaches>
+    <pivotCache cacheId="1" r:id="rId9"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="53">
   <si>
     <t>Año</t>
   </si>
@@ -141,6 +146,63 @@
   </si>
   <si>
     <t>RMSE</t>
+  </si>
+  <si>
+    <t>Etiquetas de fila</t>
+  </si>
+  <si>
+    <t>PoblacionAfrica</t>
+  </si>
+  <si>
+    <t>PoblacionAmerica</t>
+  </si>
+  <si>
+    <t>PoblacionAsia</t>
+  </si>
+  <si>
+    <t>PoblacionEuropa</t>
+  </si>
+  <si>
+    <t>PoblacionOceania</t>
+  </si>
+  <si>
+    <t>Crecimiento inferior</t>
+  </si>
+  <si>
+    <t>Crecimiento promedio</t>
+  </si>
+  <si>
+    <t>Crecimiento superior</t>
+  </si>
+  <si>
+    <t>Crecimiento por</t>
+  </si>
+  <si>
+    <t>(Todas)</t>
+  </si>
+  <si>
+    <t>Creado por Francisco Charte Ojeda el 10/02/2016</t>
+  </si>
+  <si>
+    <t>Resumen del escenario</t>
+  </si>
+  <si>
+    <t>Celdas cambiantes:</t>
+  </si>
+  <si>
+    <t>Valores actuales:</t>
+  </si>
+  <si>
+    <t>Celdas de resultado:</t>
+  </si>
+  <si>
+    <t>Notas: La columna de valores actuales representa los valores de las celdas cambiantes</t>
+  </si>
+  <si>
+    <t>en el momento en que se creó el Informe resumen de escenario. Las celdas cambiantes de</t>
+  </si>
+  <si>
+    <t>cada escenario se muestran en gris.</t>
   </si>
 </sst>
 </file>
@@ -152,7 +214,7 @@
     <numFmt numFmtId="173" formatCode="0.000E+00"/>
     <numFmt numFmtId="174" formatCode="#,##0.00\ &quot;pta&quot;;[Red]\-#,##0.00\ &quot;pta&quot;"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -186,16 +248,72 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color indexed="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="18"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="20"/>
+        <bgColor indexed="24"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="22"/>
+        <bgColor indexed="24"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="22"/>
+        <bgColor indexed="7"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -203,12 +321,50 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -244,6 +400,41 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="174" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1402,6 +1593,142 @@
 </externalLink>
 </file>
 
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="Francisco Charte Ojeda" refreshedDate="42410.541066203703" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="3">
+  <cacheSource type="scenario"/>
+  <cacheFields count="7">
+    <cacheField name="Crecimiento" numFmtId="0">
+      <sharedItems containsNonDate="0" count="3">
+        <s v="Crecimiento superior"/>
+        <s v="Crecimiento promedio"/>
+        <s v="Crecimiento inferior"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Crecimiento por" numFmtId="0">
+      <sharedItems containsNonDate="0" count="1">
+        <s v="Francisco Charte Ojeda"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="resultado PoblacionAfrica" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsString="0" containsNumber="1" minValue="770454.10499999998" maxValue="785786.52500000002" count="3">
+        <n v="785786.52500000002"/>
+        <n v="778120.31499999994"/>
+        <n v="770454.10499999998"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="resultado PoblacionAmerica" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsString="0" containsNumber="1" minValue="822537.22499999998" maxValue="838906.125" count="3">
+        <n v="838906.125"/>
+        <n v="830721.67500000005"/>
+        <n v="822537.22499999998"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="resultado PoblacionAsia" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsString="0" containsNumber="1" minValue="3652451.4" maxValue="3725137" count="3">
+        <n v="3725137"/>
+        <n v="3688794.2"/>
+        <n v="3652451.4"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="resultado PoblacionEuropa" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsString="0" containsNumber="1" minValue="743205.54" maxValue="757995.7" count="3">
+        <n v="757995.7"/>
+        <n v="750600.62"/>
+        <n v="743205.54"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="resultado PoblacionOceania" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsString="0" containsNumber="1" minValue="30165.075000000001" maxValue="30765.375" count="3">
+        <n v="30765.375"/>
+        <n v="30465.224999999999"/>
+        <n v="30165.075000000001"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Celdas de resultado" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
+  <location ref="A3:F6" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="7">
+    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
+      <items count="3">
+        <item x="2"/>
+        <item x="1"/>
+        <item x="0"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="2">
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+    <i i="2">
+      <x v="2"/>
+    </i>
+    <i i="3">
+      <x v="3"/>
+    </i>
+    <i i="4">
+      <x v="4"/>
+    </i>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="1" hier="-1"/>
+  </pageFields>
+  <dataFields count="5">
+    <dataField name="PoblacionAfrica" fld="2" baseField="0" baseItem="0"/>
+    <dataField name="PoblacionAmerica" fld="3" baseField="0" baseItem="0"/>
+    <dataField name="PoblacionAsia" fld="4" baseField="0" baseItem="0"/>
+    <dataField name="PoblacionEuropa" fld="5" baseField="0" baseItem="0"/>
+    <dataField name="PoblacionOceania" fld="6" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:D19" totalsRowShown="0">
   <autoFilter ref="A1:D19"/>
@@ -2830,8 +3157,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="A3:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2883,31 +3210,31 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
-        <v>5.0000000000000001E-3</v>
+        <v>1.52E-2</v>
       </c>
       <c r="B5" s="6">
         <f>B4*Crecimiento+B4</f>
-        <v>770454.10499999998</v>
+        <v>778273.63919999998</v>
       </c>
       <c r="C5" s="6">
         <f>C4*Crecimiento+C4</f>
-        <v>822537.22499999998</v>
+        <v>830885.36399999994</v>
       </c>
       <c r="D5" s="6">
         <f>D4*Crecimiento+D4</f>
-        <v>3652451.4</v>
+        <v>3689521.0559999999</v>
       </c>
       <c r="E5" s="6">
         <f>E4*Crecimiento+E4</f>
-        <v>743205.54</v>
+        <v>750748.52159999998</v>
       </c>
       <c r="F5" s="6">
         <f>F4*Crecimiento+F4</f>
-        <v>30165.075000000001</v>
+        <v>30471.227999999999</v>
       </c>
     </row>
   </sheetData>
-  <scenarios current="0" show="2">
+  <scenarios current="0" show="0" sqref="B5 C5 D5 E5 F5">
     <scenario name="Crecimiento superior" locked="1" count="1" user="Francisco Charte Ojeda" comment="Creado por Francisco Charte Ojeda el 10/02/2016">
       <inputCells r="A5" val="0,025" numFmtId="10"/>
     </scenario>
@@ -2920,4 +3247,319 @@
   </scenarios>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="24">
+        <v>770454.10499999998</v>
+      </c>
+      <c r="C4" s="24">
+        <v>822537.22499999998</v>
+      </c>
+      <c r="D4" s="24">
+        <v>3652451.4</v>
+      </c>
+      <c r="E4" s="24">
+        <v>743205.54</v>
+      </c>
+      <c r="F4" s="24">
+        <v>30165.075000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="24">
+        <v>778120.31499999994</v>
+      </c>
+      <c r="C5" s="24">
+        <v>830721.67500000005</v>
+      </c>
+      <c r="D5" s="24">
+        <v>3688794.2</v>
+      </c>
+      <c r="E5" s="24">
+        <v>750600.62</v>
+      </c>
+      <c r="F5" s="24">
+        <v>30465.224999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="24">
+        <v>785786.52500000002</v>
+      </c>
+      <c r="C6" s="24">
+        <v>838906.125</v>
+      </c>
+      <c r="D6" s="24">
+        <v>3725137</v>
+      </c>
+      <c r="E6" s="24">
+        <v>757995.7</v>
+      </c>
+      <c r="F6" s="24">
+        <v>30765.375</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="B1:G15"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="18.5703125" bestFit="1" customWidth="1" outlineLevel="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B2" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="30"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+    </row>
+    <row r="3" spans="2:7" ht="15.75" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" s="36" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" ht="33.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="G4" s="38" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="33"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+    </row>
+    <row r="6" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="32"/>
+      <c r="C6" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="26">
+        <v>1.52E-2</v>
+      </c>
+      <c r="E6" s="37">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="F6" s="37">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="G6" s="37">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="33"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+    </row>
+    <row r="8" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="32"/>
+      <c r="C8" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="27">
+        <v>778273.63919999998</v>
+      </c>
+      <c r="E8" s="27">
+        <v>785786.52500000002</v>
+      </c>
+      <c r="F8" s="27">
+        <v>778120.31499999994</v>
+      </c>
+      <c r="G8" s="27">
+        <v>770454.10499999998</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="32"/>
+      <c r="C9" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="27">
+        <v>830885.36399999994</v>
+      </c>
+      <c r="E9" s="27">
+        <v>838906.125</v>
+      </c>
+      <c r="F9" s="27">
+        <v>830721.67500000005</v>
+      </c>
+      <c r="G9" s="27">
+        <v>822537.22499999998</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="32"/>
+      <c r="C10" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="27">
+        <v>3689521.0559999999</v>
+      </c>
+      <c r="E10" s="27">
+        <v>3725137</v>
+      </c>
+      <c r="F10" s="27">
+        <v>3688794.2</v>
+      </c>
+      <c r="G10" s="27">
+        <v>3652451.4</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="32"/>
+      <c r="C11" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="27">
+        <v>750748.52159999998</v>
+      </c>
+      <c r="E11" s="27">
+        <v>757995.7</v>
+      </c>
+      <c r="F11" s="27">
+        <v>750600.62</v>
+      </c>
+      <c r="G11" s="27">
+        <v>743205.54</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="34"/>
+      <c r="C12" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="28">
+        <v>30471.227999999999</v>
+      </c>
+      <c r="E12" s="28">
+        <v>30765.375</v>
+      </c>
+      <c r="F12" s="28">
+        <v>30465.224999999999</v>
+      </c>
+      <c r="G12" s="28">
+        <v>30165.075000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Hoja con los informes generados por Solver
</commit_message>
<xml_diff>
--- a/05/AnalisisDatosI.xlsx
+++ b/05/AnalisisDatosI.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18105" windowHeight="10245" firstSheet="4" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18105" windowHeight="10245" firstSheet="6" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Historico población" sheetId="1" r:id="rId1"/>
@@ -19,9 +19,13 @@
     <sheet name="Escenarios" sheetId="5" r:id="rId5"/>
     <sheet name="Tabla dinámica del escenario" sheetId="6" r:id="rId6"/>
     <sheet name="Resumen del escenario" sheetId="8" r:id="rId7"/>
+    <sheet name="Solver" sheetId="9" r:id="rId8"/>
+    <sheet name="Informe de respuestas 1" sheetId="10" r:id="rId9"/>
+    <sheet name="Informe de sensibilidad 1" sheetId="11" r:id="rId10"/>
+    <sheet name="Informe de límites 1" sheetId="12" r:id="rId11"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId8"/>
+    <externalReference r:id="rId12"/>
   </externalReferences>
   <definedNames>
     <definedName name="Crecimiento">Escenarios!$A$5</definedName>
@@ -30,10 +34,51 @@
     <definedName name="PoblacionAsia">Escenarios!$D$5</definedName>
     <definedName name="PoblacionEuropa">Escenarios!$E$5</definedName>
     <definedName name="PoblacionOceania">Escenarios!$F$5</definedName>
+    <definedName name="solver_adj" localSheetId="7" hidden="1">Solver!$B$18:$F$18</definedName>
+    <definedName name="solver_cvg" localSheetId="7" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="7" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="7" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="7" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="7" hidden="1">2147483647</definedName>
+    <definedName name="solver_lhs1" localSheetId="7" hidden="1">Solver!$B$18:$F$18</definedName>
+    <definedName name="solver_lhs2" localSheetId="7" hidden="1">Solver!$D$18</definedName>
+    <definedName name="solver_mip" localSheetId="7" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="7" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="7" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="7" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="7" hidden="1">2</definedName>
+    <definedName name="solver_nod" localSheetId="7" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="4" hidden="1">0</definedName>
+    <definedName name="solver_num" localSheetId="7" hidden="1">2</definedName>
+    <definedName name="solver_nwt" localSheetId="7" hidden="1">1</definedName>
+    <definedName name="solver_opt" localSheetId="4" hidden="1">Escenarios!$G$5</definedName>
+    <definedName name="solver_opt" localSheetId="7" hidden="1">Solver!$G$19</definedName>
+    <definedName name="solver_pre" localSheetId="7" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="7" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="7" hidden="1">3</definedName>
+    <definedName name="solver_rel2" localSheetId="7" hidden="1">3</definedName>
+    <definedName name="solver_rhs1" localSheetId="7" hidden="1">0</definedName>
+    <definedName name="solver_rhs2" localSheetId="7" hidden="1">1%</definedName>
+    <definedName name="solver_rlx" localSheetId="7" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="7" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="7" hidden="1">1</definedName>
+    <definedName name="solver_sho" localSheetId="10" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="7" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="7" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="7" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="7" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_typ" localSheetId="7" hidden="1">2</definedName>
+    <definedName name="solver_val" localSheetId="4" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="7" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="4" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="7" hidden="1">3</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId9"/>
+    <pivotCache cacheId="1" r:id="rId13"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -44,7 +89,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="109">
   <si>
     <t>Año</t>
   </si>
@@ -203,6 +248,174 @@
   </si>
   <si>
     <t>cada escenario se muestran en gris.</t>
+  </si>
+  <si>
+    <t>Crecimiento continental</t>
+  </si>
+  <si>
+    <t>Microsoft Excel 16.0 Informe de respuestas</t>
+  </si>
+  <si>
+    <t>Hoja de cálculo: [AnalisisDatosI.xlsx]Solver</t>
+  </si>
+  <si>
+    <t>Informe creado: 10/02/2016 13:39:27</t>
+  </si>
+  <si>
+    <t>Resultado: Solver encontró una solución. Se cumplen todas las restricciones y condiciones óptimas.</t>
+  </si>
+  <si>
+    <t>Motor de Solver</t>
+  </si>
+  <si>
+    <t>Motor: GRG Nonlinear</t>
+  </si>
+  <si>
+    <t>Tiempo de la solución: 0,047 segundos.</t>
+  </si>
+  <si>
+    <t>Iteraciones: 6 Subproblemas: 0</t>
+  </si>
+  <si>
+    <t>Opciones de Solver</t>
+  </si>
+  <si>
+    <t>Tiempo máximo Ilimitado,  Iteraciones Ilimitado, Precision 0,000001, Usar escala automática</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Convergencia 0,0001, Tamaño de población 100, Valor de inicialización aleatorio 0, Adelantada de derivados, Requerir límites</t>
+  </si>
+  <si>
+    <t>Máximo de subproblemas Ilimitado, Máximo de soluciones de enteros Ilimitado, Tolerancia de enteros 1%</t>
+  </si>
+  <si>
+    <t>Celda objetivo (Mín)</t>
+  </si>
+  <si>
+    <t>Celda</t>
+  </si>
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Valor original</t>
+  </si>
+  <si>
+    <t>Valor final</t>
+  </si>
+  <si>
+    <t>Celdas de variables</t>
+  </si>
+  <si>
+    <t>Entero</t>
+  </si>
+  <si>
+    <t>Restricciones</t>
+  </si>
+  <si>
+    <t>Valor de la celda</t>
+  </si>
+  <si>
+    <t>Fórmula</t>
+  </si>
+  <si>
+    <t>Estado</t>
+  </si>
+  <si>
+    <t>Demora</t>
+  </si>
+  <si>
+    <t>$G$19</t>
+  </si>
+  <si>
+    <t>$B$18</t>
+  </si>
+  <si>
+    <t>Crecimiento continental África</t>
+  </si>
+  <si>
+    <t>Continuar</t>
+  </si>
+  <si>
+    <t>$C$18</t>
+  </si>
+  <si>
+    <t>Crecimiento continental América</t>
+  </si>
+  <si>
+    <t>$D$18</t>
+  </si>
+  <si>
+    <t>Crecimiento continental Asia</t>
+  </si>
+  <si>
+    <t>$E$18</t>
+  </si>
+  <si>
+    <t>Crecimiento continental Europa</t>
+  </si>
+  <si>
+    <t>$F$18</t>
+  </si>
+  <si>
+    <t>Crecimiento continental Oceanía</t>
+  </si>
+  <si>
+    <t>$B$18&gt;=0</t>
+  </si>
+  <si>
+    <t>Vinculante</t>
+  </si>
+  <si>
+    <t>$C$18&gt;=0</t>
+  </si>
+  <si>
+    <t>$D$18&gt;=0</t>
+  </si>
+  <si>
+    <t>$E$18&gt;=0</t>
+  </si>
+  <si>
+    <t>$F$18&gt;=0</t>
+  </si>
+  <si>
+    <t>Microsoft Excel 16.0 Informe de sensibilidad</t>
+  </si>
+  <si>
+    <t>Informe creado: 10/02/2016 13:39:28</t>
+  </si>
+  <si>
+    <t>Final</t>
+  </si>
+  <si>
+    <t>Reducido</t>
+  </si>
+  <si>
+    <t>Degradado</t>
+  </si>
+  <si>
+    <t>NINGUNO</t>
+  </si>
+  <si>
+    <t>Microsoft Excel 16.0 Informe de límites</t>
+  </si>
+  <si>
+    <t>Objetivo</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>Inferior</t>
+  </si>
+  <si>
+    <t>Límite</t>
+  </si>
+  <si>
+    <t>Resultado</t>
+  </si>
+  <si>
+    <t>Superior</t>
   </si>
 </sst>
 </file>
@@ -313,7 +526,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -359,12 +572,61 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="23"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="23"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="23"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="23"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="23"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="23"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="23"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -406,6 +668,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -435,6 +698,20 @@
     <xf numFmtId="10" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2571,6 +2848,378 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E16"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.28515625" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="46"/>
+      <c r="C7" s="46"/>
+      <c r="D7" s="46" t="s">
+        <v>98</v>
+      </c>
+      <c r="E7" s="46" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="47" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8" s="47" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="47" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="42" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9" s="42" t="s">
+        <v>80</v>
+      </c>
+      <c r="D9" s="42">
+        <v>0</v>
+      </c>
+      <c r="E9" s="42">
+        <v>766620.93484467966</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="D10" s="42">
+        <v>0</v>
+      </c>
+      <c r="E10" s="42">
+        <v>818445.0279458327</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="42" t="s">
+        <v>84</v>
+      </c>
+      <c r="C11" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="D11" s="42">
+        <v>0.01</v>
+      </c>
+      <c r="E11" s="42">
+        <v>3634280.0818073852</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="42" t="s">
+        <v>86</v>
+      </c>
+      <c r="C12" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="D12" s="42">
+        <v>0</v>
+      </c>
+      <c r="E12" s="42">
+        <v>739507.92561406991</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="40" t="s">
+        <v>88</v>
+      </c>
+      <c r="C13" s="40" t="s">
+        <v>89</v>
+      </c>
+      <c r="D13" s="40">
+        <v>0</v>
+      </c>
+      <c r="E13" s="40">
+        <v>30015.225482337773</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J17"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection sqref="A1:A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.28515625" customWidth="1"/>
+    <col min="2" max="2" width="6" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" customWidth="1"/>
+    <col min="4" max="4" width="5.7109375" customWidth="1"/>
+    <col min="5" max="5" width="2.28515625" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" customWidth="1"/>
+    <col min="8" max="8" width="2.28515625" customWidth="1"/>
+    <col min="9" max="9" width="8.5703125" customWidth="1"/>
+    <col min="10" max="10" width="9.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="46"/>
+      <c r="C6" s="46" t="s">
+        <v>103</v>
+      </c>
+      <c r="D6" s="46"/>
+    </row>
+    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="47" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" s="47" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="40"/>
+      <c r="D8" s="43">
+        <v>6025211.7999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="46"/>
+      <c r="C11" s="46" t="s">
+        <v>104</v>
+      </c>
+      <c r="D11" s="46"/>
+      <c r="F11" s="46" t="s">
+        <v>105</v>
+      </c>
+      <c r="G11" s="46" t="s">
+        <v>103</v>
+      </c>
+      <c r="I11" s="46" t="s">
+        <v>108</v>
+      </c>
+      <c r="J11" s="46" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" s="47" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" s="47" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" s="47" t="s">
+        <v>106</v>
+      </c>
+      <c r="G12" s="47" t="s">
+        <v>107</v>
+      </c>
+      <c r="I12" s="47" t="s">
+        <v>106</v>
+      </c>
+      <c r="J12" s="47" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="42" t="s">
+        <v>79</v>
+      </c>
+      <c r="C13" s="42" t="s">
+        <v>80</v>
+      </c>
+      <c r="D13" s="44">
+        <v>0</v>
+      </c>
+      <c r="F13" s="44">
+        <v>0</v>
+      </c>
+      <c r="G13" s="44">
+        <v>6025211.7999999998</v>
+      </c>
+      <c r="I13" s="42" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J13" s="42" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="C14" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="D14" s="44">
+        <v>0</v>
+      </c>
+      <c r="F14" s="44">
+        <v>0</v>
+      </c>
+      <c r="G14" s="44">
+        <v>6025211.7999999998</v>
+      </c>
+      <c r="I14" s="42" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J14" s="42" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="42" t="s">
+        <v>84</v>
+      </c>
+      <c r="C15" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="D15" s="44">
+        <v>0.01</v>
+      </c>
+      <c r="F15" s="44">
+        <v>0.01</v>
+      </c>
+      <c r="G15" s="44">
+        <v>6025211.7999999998</v>
+      </c>
+      <c r="I15" s="42" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J15" s="42" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="42" t="s">
+        <v>86</v>
+      </c>
+      <c r="C16" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="D16" s="44">
+        <v>0</v>
+      </c>
+      <c r="F16" s="44">
+        <v>0</v>
+      </c>
+      <c r="G16" s="44">
+        <v>6025211.7999999998</v>
+      </c>
+      <c r="I16" s="42" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J16" s="42" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="40" t="s">
+        <v>88</v>
+      </c>
+      <c r="C17" s="40" t="s">
+        <v>89</v>
+      </c>
+      <c r="D17" s="45">
+        <v>0</v>
+      </c>
+      <c r="F17" s="45">
+        <v>0</v>
+      </c>
+      <c r="G17" s="45">
+        <v>6025211.7999999998</v>
+      </c>
+      <c r="I17" s="40" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J17" s="40" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H19"/>
@@ -3155,10 +3804,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:F5"/>
+  <dimension ref="A3:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="A3:F5"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3166,7 +3815,7 @@
     <col min="1" max="1" width="19.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="11" t="s">
         <v>5</v>
       </c>
@@ -3183,7 +3832,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -3208,7 +3857,7 @@
         <v>30015</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>1.52E-2</v>
       </c>
@@ -3231,6 +3880,10 @@
       <c r="F5" s="6">
         <f>F4*Crecimiento+F4</f>
         <v>30471.227999999999</v>
+      </c>
+      <c r="G5" s="6">
+        <f>SUM(B5:F5)</f>
+        <v>6079899.8087999998</v>
       </c>
     </row>
   </sheetData>
@@ -3367,7 +4020,7 @@
   </sheetPr>
   <dimension ref="B1:G15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3377,170 +4030,170 @@
   <sheetData>
     <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
     </row>
     <row r="3" spans="2:7" ht="15.75" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="36" t="s">
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="E3" s="36" t="s">
+      <c r="E3" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="F3" s="36" t="s">
+      <c r="F3" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="G3" s="36" t="s">
+      <c r="G3" s="37" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="33.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="32"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="38" t="s">
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="F4" s="38" t="s">
+      <c r="F4" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="G4" s="38" t="s">
+      <c r="G4" s="39" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="C5" s="33"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
     </row>
     <row r="6" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="32"/>
-      <c r="C6" s="32" t="s">
+      <c r="B6" s="33"/>
+      <c r="C6" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="26">
+      <c r="D6" s="27">
         <v>1.52E-2</v>
       </c>
-      <c r="E6" s="37">
+      <c r="E6" s="38">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="F6" s="37">
+      <c r="F6" s="38">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="G6" s="37">
+      <c r="G6" s="38">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="C7" s="33"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
     </row>
     <row r="8" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="32"/>
-      <c r="C8" s="32" t="s">
+      <c r="B8" s="33"/>
+      <c r="C8" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="27">
+      <c r="D8" s="28">
         <v>778273.63919999998</v>
       </c>
-      <c r="E8" s="27">
+      <c r="E8" s="28">
         <v>785786.52500000002</v>
       </c>
-      <c r="F8" s="27">
+      <c r="F8" s="28">
         <v>778120.31499999994</v>
       </c>
-      <c r="G8" s="27">
+      <c r="G8" s="28">
         <v>770454.10499999998</v>
       </c>
     </row>
     <row r="9" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="32"/>
-      <c r="C9" s="32" t="s">
+      <c r="B9" s="33"/>
+      <c r="C9" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="27">
+      <c r="D9" s="28">
         <v>830885.36399999994</v>
       </c>
-      <c r="E9" s="27">
+      <c r="E9" s="28">
         <v>838906.125</v>
       </c>
-      <c r="F9" s="27">
+      <c r="F9" s="28">
         <v>830721.67500000005</v>
       </c>
-      <c r="G9" s="27">
+      <c r="G9" s="28">
         <v>822537.22499999998</v>
       </c>
     </row>
     <row r="10" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="32"/>
-      <c r="C10" s="32" t="s">
+      <c r="B10" s="33"/>
+      <c r="C10" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="27">
+      <c r="D10" s="28">
         <v>3689521.0559999999</v>
       </c>
-      <c r="E10" s="27">
+      <c r="E10" s="28">
         <v>3725137</v>
       </c>
-      <c r="F10" s="27">
+      <c r="F10" s="28">
         <v>3688794.2</v>
       </c>
-      <c r="G10" s="27">
+      <c r="G10" s="28">
         <v>3652451.4</v>
       </c>
     </row>
     <row r="11" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="32"/>
-      <c r="C11" s="32" t="s">
+      <c r="B11" s="33"/>
+      <c r="C11" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="27">
+      <c r="D11" s="28">
         <v>750748.52159999998</v>
       </c>
-      <c r="E11" s="27">
+      <c r="E11" s="28">
         <v>757995.7</v>
       </c>
-      <c r="F11" s="27">
+      <c r="F11" s="28">
         <v>750600.62</v>
       </c>
-      <c r="G11" s="27">
+      <c r="G11" s="28">
         <v>743205.54</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="34"/>
-      <c r="C12" s="34" t="s">
+      <c r="B12" s="35"/>
+      <c r="C12" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="28">
+      <c r="D12" s="29">
         <v>30471.227999999999</v>
       </c>
-      <c r="E12" s="28">
+      <c r="E12" s="29">
         <v>30765.375</v>
       </c>
-      <c r="F12" s="28">
+      <c r="F12" s="29">
         <v>30465.224999999999</v>
       </c>
-      <c r="G12" s="28">
+      <c r="G12" s="29">
         <v>30165.075000000001</v>
       </c>
     </row>
@@ -3562,4 +4215,529 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:G19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="6">
+        <f>[1]África!F58</f>
+        <v>766621</v>
+      </c>
+      <c r="C4" s="6">
+        <f>[1]América!F52</f>
+        <v>818445</v>
+      </c>
+      <c r="D4" s="6">
+        <f>[1]Asia!F51</f>
+        <v>3634280</v>
+      </c>
+      <c r="E4" s="6">
+        <f>[1]Europa!F47</f>
+        <v>739508</v>
+      </c>
+      <c r="F4" s="6">
+        <f>[1]Oceanía!F25</f>
+        <v>30015</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
+        <v>1.52E-2</v>
+      </c>
+      <c r="B5" s="6">
+        <f>B4*Crecimiento+B4</f>
+        <v>778273.63919999998</v>
+      </c>
+      <c r="C5" s="6">
+        <f>C4*Crecimiento+C4</f>
+        <v>830885.36399999994</v>
+      </c>
+      <c r="D5" s="6">
+        <f>D4*Crecimiento+D4</f>
+        <v>3689521.0559999999</v>
+      </c>
+      <c r="E5" s="6">
+        <f>E4*Crecimiento+E4</f>
+        <v>750748.52159999998</v>
+      </c>
+      <c r="F5" s="6">
+        <f>F4*Crecimiento+F4</f>
+        <v>30471.227999999999</v>
+      </c>
+      <c r="G5" s="6">
+        <f>SUM(B5:F5)</f>
+        <v>6079899.8087999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="25">
+        <v>0</v>
+      </c>
+      <c r="C18" s="25">
+        <v>0</v>
+      </c>
+      <c r="D18" s="25">
+        <v>0.01</v>
+      </c>
+      <c r="E18" s="25">
+        <v>0</v>
+      </c>
+      <c r="F18" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="6">
+        <f>B4*B18+B4</f>
+        <v>766621</v>
+      </c>
+      <c r="C19" s="6">
+        <f t="shared" ref="C19:F19" si="0">C4*C18+C4</f>
+        <v>818445</v>
+      </c>
+      <c r="D19" s="6">
+        <f t="shared" si="0"/>
+        <v>3670622.8</v>
+      </c>
+      <c r="E19" s="6">
+        <f t="shared" si="0"/>
+        <v>739508</v>
+      </c>
+      <c r="F19" s="6">
+        <f t="shared" si="0"/>
+        <v>30015</v>
+      </c>
+      <c r="G19" s="6">
+        <f>SUM(B19:F19)</f>
+        <v>6025211.7999999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G35"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.28515625" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" customWidth="1"/>
+    <col min="3" max="3" width="30.5703125" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" customWidth="1"/>
+    <col min="7" max="7" width="8" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="16"/>
+      <c r="B6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="16"/>
+      <c r="B7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="16"/>
+      <c r="B8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="D15" s="41" t="s">
+        <v>69</v>
+      </c>
+      <c r="E15" s="41" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="C16" s="40"/>
+      <c r="D16" s="43">
+        <v>6087663.1500000013</v>
+      </c>
+      <c r="E16" s="43">
+        <v>6025211.7999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="C20" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="D20" s="41" t="s">
+        <v>69</v>
+      </c>
+      <c r="E20" s="41" t="s">
+        <v>70</v>
+      </c>
+      <c r="F20" s="41" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="42" t="s">
+        <v>79</v>
+      </c>
+      <c r="C21" s="42" t="s">
+        <v>80</v>
+      </c>
+      <c r="D21" s="44">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="E21" s="44">
+        <v>0</v>
+      </c>
+      <c r="F21" s="42" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="C22" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="D22" s="44">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="E22" s="44">
+        <v>0</v>
+      </c>
+      <c r="F22" s="42" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="42" t="s">
+        <v>84</v>
+      </c>
+      <c r="C23" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="D23" s="44">
+        <v>0.02</v>
+      </c>
+      <c r="E23" s="44">
+        <v>0.01</v>
+      </c>
+      <c r="F23" s="42" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="42" t="s">
+        <v>86</v>
+      </c>
+      <c r="C24" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="D24" s="44">
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="E24" s="44">
+        <v>0</v>
+      </c>
+      <c r="F24" s="42" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="40" t="s">
+        <v>88</v>
+      </c>
+      <c r="C25" s="40" t="s">
+        <v>89</v>
+      </c>
+      <c r="D25" s="45">
+        <v>2E-3</v>
+      </c>
+      <c r="E25" s="45">
+        <v>0</v>
+      </c>
+      <c r="F25" s="40" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="C29" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="D29" s="41" t="s">
+        <v>74</v>
+      </c>
+      <c r="E29" s="41" t="s">
+        <v>75</v>
+      </c>
+      <c r="F29" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="G29" s="41" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="42" t="s">
+        <v>79</v>
+      </c>
+      <c r="C30" s="42" t="s">
+        <v>80</v>
+      </c>
+      <c r="D30" s="44">
+        <v>0</v>
+      </c>
+      <c r="E30" s="42" t="s">
+        <v>90</v>
+      </c>
+      <c r="F30" s="42" t="s">
+        <v>91</v>
+      </c>
+      <c r="G30" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="C31" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="D31" s="44">
+        <v>0</v>
+      </c>
+      <c r="E31" s="42" t="s">
+        <v>92</v>
+      </c>
+      <c r="F31" s="42" t="s">
+        <v>91</v>
+      </c>
+      <c r="G31" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B32" s="42" t="s">
+        <v>84</v>
+      </c>
+      <c r="C32" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="D32" s="44">
+        <v>0.01</v>
+      </c>
+      <c r="E32" s="42" t="s">
+        <v>93</v>
+      </c>
+      <c r="F32" s="42" t="s">
+        <v>91</v>
+      </c>
+      <c r="G32" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33" s="42" t="s">
+        <v>86</v>
+      </c>
+      <c r="C33" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="D33" s="44">
+        <v>0</v>
+      </c>
+      <c r="E33" s="42" t="s">
+        <v>94</v>
+      </c>
+      <c r="F33" s="42" t="s">
+        <v>91</v>
+      </c>
+      <c r="G33" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34" s="42" t="s">
+        <v>88</v>
+      </c>
+      <c r="C34" s="42" t="s">
+        <v>89</v>
+      </c>
+      <c r="D34" s="44">
+        <v>0</v>
+      </c>
+      <c r="E34" s="42" t="s">
+        <v>95</v>
+      </c>
+      <c r="F34" s="42" t="s">
+        <v>91</v>
+      </c>
+      <c r="G34" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="40" t="s">
+        <v>84</v>
+      </c>
+      <c r="C35" s="40" t="s">
+        <v>85</v>
+      </c>
+      <c r="D35" s="45">
+        <v>0.01</v>
+      </c>
+      <c r="E35" s="40" t="s">
+        <v>93</v>
+      </c>
+      <c r="F35" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="G35" s="45">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>